<commit_message>
Udacity PBI Project 1 Update
</commit_message>
<xml_diff>
--- a/Step 2_Structure Combine and Clean the Data.xlsx
+++ b/Step 2_Structure Combine and Clean the Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Udacity_PBI\Project_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39309EA8-EEA8-44E4-BA5A-23FED3A6DC1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F2FC37-3385-49F9-88D6-BA67279820E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="2" xr2:uid="{54E99262-162D-48F5-9BA6-60E490621784}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="14020" activeTab="1" xr2:uid="{54E99262-162D-48F5-9BA6-60E490621784}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="33">
   <si>
     <t>File</t>
   </si>
@@ -92,9 +92,6 @@
     <t>Yes - CAD in the May 2021 spreadsheet</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>Merge Dimension Tables</t>
   </si>
   <si>
@@ -129,6 +126,15 @@
   </si>
   <si>
     <t>Yes - 16 rows</t>
+  </si>
+  <si>
+    <t>Yes - 2 rows where PKProductID is null</t>
+  </si>
+  <si>
+    <t>Consider drop Description?</t>
+  </si>
+  <si>
+    <t>Yes in import some unlabelled</t>
   </si>
 </sst>
 </file>
@@ -499,7 +505,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,7 +593,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
@@ -621,71 +627,90 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BD5A9EC-F10D-4F62-B61E-184E978B341F}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>7</v>
       </c>
     </row>
@@ -699,16 +724,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2039BB1D-859A-4CFE-B18D-90C7F36CADE1}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27.26953125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.26953125" customWidth="1"/>
-    <col min="3" max="3" width="29.1796875" customWidth="1"/>
-    <col min="4" max="4" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" customWidth="1"/>
     <col min="5" max="5" width="14.90625" customWidth="1"/>
     <col min="6" max="6" width="21.08984375" customWidth="1"/>
   </cols>
@@ -718,19 +743,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -741,16 +766,16 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -761,16 +786,16 @@
         <v>14</v>
       </c>
       <c r="C3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
         <v>27</v>
       </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>28</v>
-      </c>
-      <c r="F3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -781,13 +806,16 @@
         <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4" t="s">
-        <v>27</v>
+        <v>26</v>
+      </c>
+      <c r="F4" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -797,6 +825,18 @@
       <c r="B5" s="2" t="s">
         <v>11</v>
       </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -804,6 +844,18 @@
       </c>
       <c r="B6" t="s">
         <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F6" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>